<commit_message>
Add manual scripts and adjusted sliders
</commit_message>
<xml_diff>
--- a/Tabelas Scripts Rebranding.xlsx
+++ b/Tabelas Scripts Rebranding.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="157">
   <si>
     <t xml:space="preserve">tabelas</t>
   </si>
@@ -449,6 +449,9 @@
     <t xml:space="preserve">status não é mais boolean, mas "published" and "draft" **fazer insert tbm</t>
   </si>
   <si>
+    <t xml:space="preserve">existem seeders para os menus novos</t>
+  </si>
+  <si>
     <t xml:space="preserve">meta_boxes</t>
   </si>
   <si>
@@ -477,6 +480,9 @@
   </si>
   <si>
     <t xml:space="preserve">algumas colunas foram adicionadas no rebranding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">menu_nodes verificar se precisar inserir novos menus, creio que sim</t>
   </si>
   <si>
     <t xml:space="preserve">Aline, vc é fera</t>
@@ -611,7 +617,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -700,20 +706,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -726,6 +724,22 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -805,13 +819,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I112" activeCellId="0" sqref="I112"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A117" activeCellId="0" sqref="A117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
@@ -2558,99 +2572,108 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="5" t="s">
+      <c r="A110" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B110" s="21"/>
-      <c r="C110" s="21"/>
-      <c r="D110" s="21"/>
-      <c r="E110" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F110" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G110" s="22" t="s">
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G110" s="17" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="23" t="s">
+      <c r="H110" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B111" s="24"/>
-      <c r="C111" s="24"/>
-      <c r="D111" s="24"/>
-      <c r="E111" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F111" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="G111" s="24" t="s">
+    </row>
+    <row r="111" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="3" t="s">
         <v>143</v>
       </c>
+      <c r="B111" s="22"/>
+      <c r="C111" s="22"/>
+      <c r="D111" s="22"/>
+      <c r="E111" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F111" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G111" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="J111" s="3"/>
     </row>
     <row r="112" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="B112" s="21"/>
-      <c r="C112" s="21"/>
-      <c r="D112" s="21"/>
-      <c r="E112" s="21"/>
-      <c r="F112" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G112" s="22" t="s">
+      <c r="A112" s="20" t="s">
         <v>145</v>
       </c>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G112" s="17" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="B113" s="21"/>
-      <c r="C113" s="21"/>
-      <c r="D113" s="21"/>
-      <c r="E113" s="21"/>
-      <c r="F113" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G113" s="22" t="s">
+      <c r="A113" s="20" t="s">
         <v>147</v>
       </c>
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G113" s="17" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="B114" s="21"/>
-      <c r="C114" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D114" s="21"/>
-      <c r="E114" s="21"/>
-      <c r="F114" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G114" s="21" t="s">
+      <c r="A114" s="3" t="s">
         <v>149</v>
       </c>
+      <c r="B114" s="4"/>
+      <c r="C114" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G114" s="4" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B115" s="21"/>
-      <c r="C115" s="21"/>
-      <c r="D115" s="21"/>
-      <c r="E115" s="21"/>
-      <c r="F115" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G115" s="21" t="s">
+      <c r="A115" s="3" t="s">
         <v>151</v>
+      </c>
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G115" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2675,14 +2698,14 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="26" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="26" width="19.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="26" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="26" width="65.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="24" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="24" width="19.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="24" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="24" width="65.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="40.28"/>
   </cols>
   <sheetData>
@@ -2805,18 +2828,18 @@
       <c r="A7" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27" t="s">
+      <c r="B7" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25" t="s">
         <v>100</v>
       </c>
       <c r="I7" s="9"/>
@@ -2853,7 +2876,7 @@
       <c r="G9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="26" t="s">
         <v>126</v>
       </c>
       <c r="B10" s="21"/>
@@ -2863,11 +2886,11 @@
       <c r="F10" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="27" t="s">
         <v>127</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3182,16 +3205,16 @@
       <c r="A31" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27" t="s">
+      <c r="B31" s="25"/>
+      <c r="C31" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3199,16 +3222,16 @@
       <c r="A32" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27" t="s">
+      <c r="B32" s="25"/>
+      <c r="C32" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3271,7 +3294,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="28" t="s">
         <v>133</v>
       </c>
       <c r="B37" s="21"/>
@@ -3281,7 +3304,7 @@
       <c r="F37" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G37" s="22" t="s">
+      <c r="G37" s="27" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3653,25 +3676,25 @@
       <c r="F59" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G59" s="22" t="s">
+      <c r="G59" s="27" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
+      <c r="A60" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="B60" s="30"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
       <c r="E60" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F60" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="G60" s="24" t="s">
-        <v>143</v>
+      <c r="F60" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60" s="30" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3923,8 +3946,8 @@
       <c r="G76" s="13"/>
     </row>
     <row r="77" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="25" t="s">
-        <v>144</v>
+      <c r="A77" s="28" t="s">
+        <v>145</v>
       </c>
       <c r="B77" s="21"/>
       <c r="C77" s="21"/>
@@ -3933,8 +3956,8 @@
       <c r="F77" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G77" s="22" t="s">
-        <v>145</v>
+      <c r="G77" s="27" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3975,14 +3998,14 @@
       <c r="A80" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B80" s="27"/>
-      <c r="C80" s="27"/>
-      <c r="D80" s="27"/>
-      <c r="E80" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F80" s="27"/>
-      <c r="G80" s="27" t="s">
+      <c r="B80" s="25"/>
+      <c r="C80" s="25"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="25"/>
+      <c r="G80" s="25" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3990,14 +4013,14 @@
       <c r="A81" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B81" s="27"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F81" s="27"/>
-      <c r="G81" s="27" t="s">
+      <c r="B81" s="25"/>
+      <c r="C81" s="25"/>
+      <c r="D81" s="25"/>
+      <c r="E81" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="25"/>
+      <c r="G81" s="25" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4005,14 +4028,14 @@
       <c r="A82" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B82" s="27"/>
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F82" s="27"/>
-      <c r="G82" s="27" t="s">
+      <c r="B82" s="25"/>
+      <c r="C82" s="25"/>
+      <c r="D82" s="25"/>
+      <c r="E82" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="25"/>
+      <c r="G82" s="25" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4020,14 +4043,14 @@
       <c r="A83" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B83" s="27"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F83" s="27"/>
-      <c r="G83" s="27" t="s">
+      <c r="B83" s="25"/>
+      <c r="C83" s="25"/>
+      <c r="D83" s="25"/>
+      <c r="E83" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="25"/>
+      <c r="G83" s="25" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4035,14 +4058,14 @@
       <c r="A84" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B84" s="27"/>
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F84" s="27"/>
-      <c r="G84" s="27" t="s">
+      <c r="B84" s="25"/>
+      <c r="C84" s="25"/>
+      <c r="D84" s="25"/>
+      <c r="E84" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="25"/>
+      <c r="G84" s="25" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4060,7 +4083,7 @@
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4288,7 +4311,7 @@
       <c r="E101" s="21"/>
       <c r="F101" s="21"/>
       <c r="G101" s="21" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4324,8 +4347,8 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="25" t="s">
-        <v>146</v>
+      <c r="A104" s="28" t="s">
+        <v>147</v>
       </c>
       <c r="B104" s="21"/>
       <c r="C104" s="21"/>
@@ -4334,8 +4357,8 @@
       <c r="F104" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G104" s="22" t="s">
-        <v>147</v>
+      <c r="G104" s="27" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4353,7 +4376,7 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B106" s="21"/>
       <c r="C106" s="21" t="s">
@@ -4365,7 +4388,7 @@
         <v>9</v>
       </c>
       <c r="G106" s="21" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4419,7 +4442,7 @@
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B110" s="21"/>
       <c r="C110" s="21"/>
@@ -4429,7 +4452,7 @@
         <v>9</v>
       </c>
       <c r="G110" s="21" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>